<commit_message>
Minor Change to main, DataMatrix and DataMatrixInformation & added Multiplier file
</commit_message>
<xml_diff>
--- a/DataMatrix.xlsx
+++ b/DataMatrix.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Neamen\Google Drive\Senior Design_\PMDK\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\Documents\SchoolStuff\Senior Design\Senior-Design-\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -168,23 +168,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -220,23 +203,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -391,13 +357,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BI10" sqref="BI10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -585,7 +551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -773,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -961,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1146,11 +1112,10 @@
         <v>0</v>
       </c>
       <c r="BJ4" s="1">
-        <f ca="1">+BA4:BJ4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0</v>
       </c>
@@ -1338,7 +1303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -1526,7 +1491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>1</v>
       </c>
@@ -1714,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1</v>
       </c>
@@ -1902,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -2090,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>0</v>
       </c>

</xml_diff>